<commit_message>
Updated code with bug fixing and implement feedback changes
</commit_message>
<xml_diff>
--- a/AttendanceManagement/wwwroot/ExcelTemplates/Probation Report.xlsx
+++ b/AttendanceManagement/wwwroot/ExcelTemplates/Probation Report.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28816"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29203"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{460F7D02-5F38-4B8E-B489-3BA63F9CAD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7844C1C-936C-4DDC-8CE9-19E89091536A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Emp ID</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Production Achieved % Dec</t>
+  </si>
+  <si>
+    <t>No Of Months</t>
   </si>
 </sst>
 </file>
@@ -493,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB1"/>
+  <dimension ref="A1:AC1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AJ12" sqref="AJ12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -522,9 +525,10 @@
     <col min="24" max="25" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="24" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -608,6 +612,9 @@
       </c>
       <c r="AB1" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated code with fixing bugs and feedbacks
</commit_message>
<xml_diff>
--- a/AttendanceManagement/wwwroot/ExcelTemplates/Probation Report.xlsx
+++ b/AttendanceManagement/wwwroot/ExcelTemplates/Probation Report.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28816"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29203"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{460F7D02-5F38-4B8E-B489-3BA63F9CAD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7844C1C-936C-4DDC-8CE9-19E89091536A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Emp ID</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Production Achieved % Dec</t>
+  </si>
+  <si>
+    <t>No Of Months</t>
   </si>
 </sst>
 </file>
@@ -493,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB1"/>
+  <dimension ref="A1:AC1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AJ12" sqref="AJ12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -522,9 +525,10 @@
     <col min="24" max="25" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="24" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -608,6 +612,9 @@
       </c>
       <c r="AB1" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>